<commit_message>
corrected data for fm12
</commit_message>
<xml_diff>
--- a/validation/insurance_fm/combine_location_w_formula.xlsx
+++ b/validation/insurance_fm/combine_location_w_formula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_branch\validation\insurance_fm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789DD92C-68EB-488C-8762-6E456C487A1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADEA0F3-4D94-4C2D-91EC-45B12FF69C2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AA4BAE3-08AC-4DFB-A8E6-9FDCEC5EA9D9}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>PortNumber</t>
   </si>
@@ -310,6 +310,12 @@
   <si>
     <t>LocLimitType2Other</t>
   </si>
+  <si>
+    <t>LocMinDed6All</t>
+  </si>
+  <si>
+    <t>LocMaxDed6All</t>
+  </si>
 </sst>
 </file>
 
@@ -7984,7 +7990,7 @@
       <sheetName val="location"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
+      <sheetData sheetId="0">
         <row r="1">
           <cell r="A1" t="str">
             <v>PortNumber</v>
@@ -11863,10 +11869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536FC415-5BB6-405B-87B6-FE54E8C2F3AA}">
-  <dimension ref="A1:BP63"/>
+  <dimension ref="A1:BR63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC36" workbookViewId="0">
-      <selection activeCell="BM1" sqref="BM1:BP63"/>
+    <sheetView tabSelected="1" topLeftCell="G8" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15:W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11933,7 +11939,7 @@
     <col min="64" max="64" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -12135,8 +12141,14 @@
       <c r="BP1" t="s">
         <v>83</v>
       </c>
+      <c r="BQ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -12407,8 +12419,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[1]location!$A$1:$X$100,$B2,FALSE),0)</f>
         <v>90000</v>
       </c>
+      <c r="BQ2">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[1]location!$A$1:$X$100,$B2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[1]location!$A$1:$X$100,$B2,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -12679,8 +12699,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[2]location!$A$1:$DC$100,$B3,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ3">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[2]location!$A$1:$DC$100,$B3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR3">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[2]location!$A$1:$DC$100,$B3,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -12951,8 +12979,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[3]location!$A$1:$DC$100,$B4,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ4">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[3]location!$A$1:$DC$100,$B4,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR4">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[3]location!$A$1:$DC$100,$B4,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -13223,8 +13259,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[4]location!$A$1:$DC$100,$B5,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ5">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[4]location!$A$1:$DC$100,$B5,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR5">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[4]location!$A$1:$DC$100,$B5,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -13495,8 +13539,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[4]location!$A$1:$DC$100,$B6,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ6">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[4]location!$A$1:$DC$100,$B6,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR6">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[4]location!$A$1:$DC$100,$B6,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -13767,8 +13819,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[5]location!$A$1:$DC$100,$B7,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ7">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[5]location!$A$1:$DC$100,$B7,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR7">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[5]location!$A$1:$DC$100,$B7,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -14039,8 +14099,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[5]location!$A$1:$DC$100,$B8,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ8">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[5]location!$A$1:$DC$100,$B8,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR8">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[5]location!$A$1:$DC$100,$B8,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -14311,8 +14379,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[6]location!$A$1:$AX$100,$B9,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ9">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[6]location!$A$1:$AX$100,$B9,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR9">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[6]location!$A$1:$AX$100,$B9,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -14583,8 +14659,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[6]location!$A$1:$AX$100,$B10,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ10">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[6]location!$A$1:$AX$100,$B10,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR10">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[6]location!$A$1:$AX$100,$B10,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -14855,8 +14939,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[7]location!$A$1:$AX$100,$B11,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ11">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[7]location!$A$1:$AX$100,$B11,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR11">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[7]location!$A$1:$AX$100,$B11,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -15127,8 +15219,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[7]location!$A$1:$AX$100,$B12,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ12">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[7]location!$A$1:$AX$100,$B12,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR12">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[7]location!$A$1:$AX$100,$B12,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -15399,8 +15499,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[8]location!$A$1:$AX$100,$B13,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ13">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[8]location!$A$1:$AX$100,$B13,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR13">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[8]location!$A$1:$AX$100,$B13,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -15671,8 +15779,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[8]location!$A$1:$AX$100,$B14,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ14">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[8]location!$A$1:$AX$100,$B14,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR14">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[8]location!$A$1:$AX$100,$B14,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -15943,8 +16059,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B15,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ15">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B15,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR15">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B15,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -16215,8 +16339,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B16,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ16">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B16,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR16">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B16,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -16487,8 +16619,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B17,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ17">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B17,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR17">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B17,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -16759,8 +16899,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B18,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ18">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B18,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR18">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B18,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -17031,8 +17179,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B19,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ19">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B19,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR19">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B19,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -17303,8 +17459,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B20,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ20">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B20,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR20">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B20,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -17575,8 +17739,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B21,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ21">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B21,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR21">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B21,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -17847,8 +18019,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B22,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ22">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B22,FALSE),0)</f>
+        <v>25000</v>
+      </c>
+      <c r="BR22">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B22,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -18119,8 +18299,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B23,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ23">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B23,FALSE),0)</f>
+        <v>25000</v>
+      </c>
+      <c r="BR23">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B23,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -18391,8 +18579,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B24,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ24">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B24,FALSE),0)</f>
+        <v>25000</v>
+      </c>
+      <c r="BR24">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B24,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -18663,8 +18859,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B25,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ25">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B25,FALSE),0)</f>
+        <v>78783.03</v>
+      </c>
+      <c r="BR25">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B25,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -18935,8 +19139,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B26,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ26">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B26,FALSE),0)</f>
+        <v>25000</v>
+      </c>
+      <c r="BR26">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B26,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -19207,8 +19419,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B27,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ27">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B27,FALSE),0)</f>
+        <v>89642.04</v>
+      </c>
+      <c r="BR27">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B27,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -19479,8 +19699,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B28,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ28">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B28,FALSE),0)</f>
+        <v>25000</v>
+      </c>
+      <c r="BR28">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B28,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -19751,8 +19979,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B29,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ29">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B29,FALSE),0)</f>
+        <v>85681.982999999993</v>
+      </c>
+      <c r="BR29">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B29,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -20023,8 +20259,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B30,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ30">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B30,FALSE),0)</f>
+        <v>140183.82</v>
+      </c>
+      <c r="BR30">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B30,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -20295,8 +20539,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B31,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ31">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B31,FALSE),0)</f>
+        <v>25000</v>
+      </c>
+      <c r="BR31">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B31,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -20567,8 +20819,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[9]location!$A$1:$DC$100,$B32,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ32">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[9]location!$A$1:$DC$100,$B32,FALSE),0)</f>
+        <v>462684.45</v>
+      </c>
+      <c r="BR32">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[9]location!$A$1:$DC$100,$B32,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -20839,8 +21099,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[10]location!$A$1:$AX$100,$B33,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ33">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[10]location!$A$1:$AX$100,$B33,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR33">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[10]location!$A$1:$AX$100,$B33,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -21111,8 +21379,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[11]location!$A$1:$AX$100,$B34,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ34">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[11]location!$A$1:$AX$100,$B34,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR34">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[11]location!$A$1:$AX$100,$B34,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -21383,8 +21659,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[11]location!$A$1:$AX$100,$B35,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ35">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[11]location!$A$1:$AX$100,$B35,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR35">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[11]location!$A$1:$AX$100,$B35,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -21655,8 +21939,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[12]location!$A$1:$AX$100,$B36,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ36">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[12]location!$A$1:$AX$100,$B36,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR36">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[12]location!$A$1:$AX$100,$B36,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -21927,8 +22219,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[12]location!$A$1:$AX$100,$B37,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ37">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[12]location!$A$1:$AX$100,$B37,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR37">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[12]location!$A$1:$AX$100,$B37,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -22199,8 +22499,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[13]location!$A$1:$AX$100,$B38,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ38">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[13]location!$A$1:$AX$100,$B38,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR38">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[13]location!$A$1:$AX$100,$B38,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -22471,8 +22779,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[13]location!$A$1:$AX$100,$B39,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ39">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[13]location!$A$1:$AX$100,$B39,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR39">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[13]location!$A$1:$AX$100,$B39,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -22743,8 +23059,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[14]location!$A$1:$AX$100,$B40,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ40">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[14]location!$A$1:$AX$100,$B40,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR40">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[14]location!$A$1:$AX$100,$B40,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -23015,8 +23339,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[14]location!$A$1:$AX$100,$B41,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ41">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[14]location!$A$1:$AX$100,$B41,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR41">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[14]location!$A$1:$AX$100,$B41,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -23287,8 +23619,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[15]location!$A$1:$AX$100,$B42,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ42">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[15]location!$A$1:$AX$100,$B42,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR42">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[15]location!$A$1:$AX$100,$B42,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -23559,8 +23899,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[15]location!$A$1:$AX$100,$B43,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ43">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[15]location!$A$1:$AX$100,$B43,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR43">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[15]location!$A$1:$AX$100,$B43,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -23831,8 +24179,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[16]location!$A$1:$AX$100,$B44,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ44">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[16]location!$A$1:$AX$100,$B44,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR44">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[16]location!$A$1:$AX$100,$B44,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -24103,8 +24459,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[16]location!$A$1:$AX$100,$B45,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ45">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[16]location!$A$1:$AX$100,$B45,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR45">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[16]location!$A$1:$AX$100,$B45,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -24375,8 +24739,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[16]location!$A$1:$AX$100,$B46,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ46">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[16]location!$A$1:$AX$100,$B46,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR46">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[16]location!$A$1:$AX$100,$B46,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -24647,8 +25019,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[16]location!$A$1:$AX$100,$B47,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ47">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[16]location!$A$1:$AX$100,$B47,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR47">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[16]location!$A$1:$AX$100,$B47,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -24919,8 +25299,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[16]location!$A$1:$AX$100,$B48,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ48">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[16]location!$A$1:$AX$100,$B48,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR48">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[16]location!$A$1:$AX$100,$B48,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -25191,8 +25579,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[16]location!$A$1:$AX$100,$B49,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ49">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[16]location!$A$1:$AX$100,$B49,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR49">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[16]location!$A$1:$AX$100,$B49,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -25463,8 +25859,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[17]location!$A$1:$AX$100,$B50,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ50">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[17]location!$A$1:$AX$100,$B50,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR50">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[17]location!$A$1:$AX$100,$B50,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -25735,8 +26139,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[17]location!$A$1:$AX$100,$B51,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ51">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[17]location!$A$1:$AX$100,$B51,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR51">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[17]location!$A$1:$AX$100,$B51,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -26007,8 +26419,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[17]location!$A$1:$AX$100,$B52,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ52">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[17]location!$A$1:$AX$100,$B52,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR52">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[17]location!$A$1:$AX$100,$B52,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -26279,8 +26699,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[17]location!$A$1:$AX$100,$B53,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ53">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[17]location!$A$1:$AX$100,$B53,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR53">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[17]location!$A$1:$AX$100,$B53,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -26551,8 +26979,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[17]location!$A$1:$AX$100,$B54,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ54">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[17]location!$A$1:$AX$100,$B54,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR54">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[17]location!$A$1:$AX$100,$B54,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -26823,8 +27259,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[17]location!$A$1:$AX$100,$B55,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ55">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[17]location!$A$1:$AX$100,$B55,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR55">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[17]location!$A$1:$AX$100,$B55,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -27095,8 +27539,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B56,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ56">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B56,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR56">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B56,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -27367,8 +27819,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B57,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ57">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B57,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR57">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B57,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>80</v>
       </c>
@@ -27639,8 +28099,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B58,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ58">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B58,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR58">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B58,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -27911,8 +28379,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B59,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ59">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B59,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR59">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B59,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -28183,8 +28659,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B60,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ60">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B60,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR60">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B60,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -28455,8 +28939,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B61,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ61">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B61,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR61">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B61,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -28727,8 +29219,16 @@
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B62,FALSE),0)</f>
         <v>0</v>
       </c>
+      <c r="BQ62">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B62,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR62">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B62,FALSE),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -28997,6 +29497,14 @@
       </c>
       <c r="BP63">
         <f>_xlfn.IFNA(HLOOKUP(BP$1,[18]location!$A$1:$AX$100,$B63,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ63">
+        <f>_xlfn.IFNA(HLOOKUP(BQ$1,[18]location!$A$1:$AX$100,$B63,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR63">
+        <f>_xlfn.IFNA(HLOOKUP(BR$1,[18]location!$A$1:$AX$100,$B63,FALSE),0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>